<commit_message>
Bank of America TestCases
</commit_message>
<xml_diff>
--- a/com.bankofamerica/src/test/resources/test_data.xlsx
+++ b/com.bankofamerica/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malik/IdeaProjects/Team1SeleniumBootcamp/com.bankofamerica/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A2AE5A-1FB7-784E-A2A1-E078D054CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A908CA8-BDB7-E845-9E33-4F1D0C8C2FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{67AED122-A9B0-F949-A52B-97840948F539}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{67AED122-A9B0-F949-A52B-97840948F539}"/>
   </bookViews>
   <sheets>
     <sheet name="BOA_sheet" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Checking</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Open an account that fits your needs</t>
+  </si>
+  <si>
+    <t>Merrill Guided Investing4</t>
+  </si>
+  <si>
+    <t>Review our Online Privacy Notice</t>
+  </si>
+  <si>
+    <t>Your security is our top priority</t>
   </si>
 </sst>
 </file>
@@ -95,8 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086104EF-2A03-4D4B-8162-AD1BFC306D36}">
-  <dimension ref="A2:A11"/>
+  <dimension ref="A2:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -472,6 +484,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>